<commit_message>
Changes in the combo chart
</commit_message>
<xml_diff>
--- a/template/charts.xlsx
+++ b/template/charts.xlsx
@@ -1,21 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27417"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11208"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dimas/projects/xlsx-chart/template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tisharakodithuwakku/Desktop/Projects/xlsx_chart/xlsx-chart/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{99F7B61C-2714-394E-999B-55FE19E00B48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart" sheetId="1" r:id="rId1"/>
     <sheet name="Table" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" concurrentCalc="0"/>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Table!$A$2:$A$4</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Table!$B$1</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Table!$B$1</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Table!$B$2:$B$4</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Table!$C$1</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Table!$C$2:$C$4</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">Table!$D$1</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">Table!$D$2:$D$4</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">Table!$E$1</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">Table!$E$2:$E$4</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Table!$B$2:$B$4</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Table!$C$1</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Table!$C$2:$C$4</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Table!$D$1</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Table!$D$2:$D$4</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Table!$E$1</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Table!$E$2:$E$4</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Table!$A$2:$A$4</definedName>
+  </definedNames>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -54,7 +75,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -89,7 +110,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -97,14 +118,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="ru-RU"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -118,70 +142,6 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:areaChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Table!$E$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>org4</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>Table!$A$2:$A$4</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>attr1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>attr2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>attr3</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Table!$E$2:$E$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>12.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>14.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>19.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="2024119312"/>
-        <c:axId val="2024123312"/>
-      </c:areaChart>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -225,17 +185,78 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-437E-FE49-B527-1A883B7E67F4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Table!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>org2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Table!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>attr1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>attr2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>attr3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Table!$C$2:$C$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-437E-FE49-B527-1A883B7E67F4}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -249,73 +270,6 @@
         <c:axId val="2024119312"/>
         <c:axId val="2024123312"/>
       </c:barChart>
-      <c:barChart>
-        <c:barDir val="bar"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Table!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>org2</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Table!$A$2:$A$4</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>attr1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>attr2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>attr3</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Table!$C$2:$C$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>15.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>20.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="2024130800"/>
-        <c:axId val="2024126992"/>
-      </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -360,18 +314,82 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>35.0</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-437E-FE49-B527-1A883B7E67F4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Table!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>org4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Table!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>attr1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>attr2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>attr3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Table!$E$2:$E$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-437E-FE49-B527-1A883B7E67F4}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -383,8 +401,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2024119312"/>
-        <c:axId val="2024123312"/>
+        <c:axId val="721499903"/>
+        <c:axId val="722147855"/>
       </c:lineChart>
       <c:catAx>
         <c:axId val="2024119312"/>
@@ -421,33 +439,32 @@
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2024126992"/>
+        <c:axId val="722147855"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="t"/>
+        <c:axPos val="r"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2024130800"/>
+        <c:crossAx val="721499903"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="2024130800"/>
+        <c:axId val="721499903"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
-        <c:axPos val="l"/>
+        <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2024126992"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="722147855"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -456,7 +473,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -488,7 +504,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Диаграмма 1"/>
+        <xdr:cNvPr id="2" name="Диаграмма 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -792,10 +814,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
@@ -807,10 +829,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>

</xml_diff>